<commit_message>
new scripts for icdc new study and data
</commit_message>
<xml_diff>
--- a/InputFiles/TC04_Canine_Filter_Study-UBC.xlsx
+++ b/InputFiles/TC04_Canine_Filter_Study-UBC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E838CAF-34EB-41F6-AAAD-03747A0B1404}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDBA4FA3-792C-4983-9E93-E104904CDAE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -77,22 +77,6 @@
         coalesce(co.cohort_description, '') AS `Cohort`</t>
   </si>
   <si>
-    <t>MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
- MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
-WHERE s.clinical_study_designation IN ['UBC01']
-WITH DISTINCT f, parent, c, demo, diag, s
-RETURN coalesce(f.file_name, '') AS `File Name`, 
-        coalesce(labels(parent)[0], '') AS `Association`,
-        coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
 WHERE s.clinical_study_designation IN ['UBC01']
 WITH DISTINCT samp AS samp, c, demo, diag
@@ -126,6 +110,24 @@
 	count(DISTINCT(samp)) as number_of_sample , 
 	count(DISTINCT(c.case_id)) as number_of_cases , 
 	count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+ MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
+WHERE s.clinical_study_designation IN ['UBC01']
+WITH DISTINCT f, parent, c, demo, diag, s
+RETURN coalesce(f.file_name, '') AS `File Name`, 
+        coalesce(f.file_type, '') AS `File Type`, 
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`,
+        coalesce(f.file_format, '') AS `File Format`,
+        coalesce(f.file_size, '') AS `Size`,
+        coalesce(c.case_id, '') AS `Case ID`, 
+        coalesce(demo.breed,'') AS Breed , 
+        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
   </si>
 </sst>
 </file>
@@ -497,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -534,13 +536,13 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="232" x14ac:dyDescent="0.35">
@@ -548,33 +550,33 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="4" spans="1:5" ht="203" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>